<commit_message>
Add 11 missing rules from review matrix to buckets file
Added rules with appropriate bucket mappings:
- Aircraft -> AIRCRAFT (unit type)
- Armor(X) -> ARMOR (defense)
- Artillery -> ARTILLERY (unit type)
- Energy Shield -> REGENERATION (similar ignore wound effect)
- Ignores Cover when Shooting -> BUCKET_003 (same as Indirect)
- Ignores Regeneration in Melee -> BUCKET_002 (same as Bane)
- Immobile -> IMMOBILE (movement)
- Massive Spores -> SPORES (faction-specific)
- Precision -> SNIPER (similar targeting effect)
- Spores -> SPORES (faction-specific)
- Transport(X) -> TRANSPORT (unit type)

Now all 516 rules from review matrix have bucket assignments.
</commit_message>
<xml_diff>
--- a/docs/special_rules_buckets.xlsx
+++ b/docs/special_rules_buckets.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Rules_With_Buckets" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Bucket_Summary" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N506"/>
+  <dimension ref="A1:N528"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25526,2653 +25525,1149 @@
       <c r="M506" t="inlineStr"/>
       <c r="N506" t="inlineStr"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I67"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Bucket_ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Rule_Count</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Rules</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Effect_Type</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Effect_Value</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Trigger_Step</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Trigger_Condition</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Grants_Rule</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Phases</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BUCKET_021</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>46</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>BOUNDING_AURA, CLAN_WARRIOR_BOOST_AURA, COORDINATE, COUNTER_ATTACK_AURA, DEFENSIVE_GROWTH_AURA, DELAYED_ACTION, DEVOUT_BOOST_AURA, EVASIVE_AURA, FEROCIOUS_BOOST_AURA, FORTIFIED_AURA, GROUNDED_PRECISION_AURA, GROUNDED_REINFORCEMENT_AURA, GUARDIAN_BOOST_AURA, GUERRILLA_BOOST_AURA, HARASSING_BOOST_AURA, HAVOCBOUND_BOOST_AURA, HIGHBORN_BOOST_AURA, HIVE_BOND_BOOST_AURA, HOLD_THE_LINE_BOOST_AURA, INFECTED_BOOST_AURA, LUSTBOUND_BOOST_AURA, MACHINE_FOG_BOOST_AURA, MISCHIEVOUS_BOOST_AURA, NO_RETREAT_AURA, PIERCING_ASSAULT_AURA, PIERCING_HUNTER_AURA, PLAGUEBOUND_BOOST_AURA, POINT_BLANK_PIERCING_AURA, QUICK_SHOT_AURA, RAPID_BLINK_BOOST_AURA, REANIMATION_AURA, REGENERATION_AURA, RESISTANCE_AURA, SCRAPPER_BOOST_AURA, SCURRY_BOOST_AURA, SPEED_FEAT_AURA, SPELL_ACCUMULATOR, STEALTH_AURA, STURDY_BOOST_AURA, SWIFT_AURA, TARGETING_VISOR_BOOST_AURA, TELEPORT_AURA, VENGEANCE, VERSATILE_DEFENSE_AURA, VERSATILE_REACH_AURA, WARBOUND_BOOST_AURA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>BUCKET_013</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>14</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>BANE_WHEN_SHOOTING_AURA, EXTENDED_BUFF_RANGE, HIT_RUN_SHOOTER_AURA, INCREASED_SHOOTING_RANGE, INCREASED_SHOOTING_RANGE_AURA, INDIRECT_WHEN_SHOOTING_AURA, QUAKE_WHEN_SHOOTING, QUICK_READJUSTMENT, RANGED_SHROUDING_AURA, RANGED_SLAYER_AURA, RENDING_WHEN_SHOOTING_AURA, SHRED_WHEN_SHOOTING_AURA, UNPREDICTABLE_SHOOTER_AURA, UNSTOPPABLE_WHEN_SHOOTING_AURA</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>BUCKET_029</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>13</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CHANGEBOUND_BOOST_AURA, DEVOUT_BOOST, FEROCIOUS_BOOST, INFECTED, LACERATE, MISCHIEVOUS, RAPID_BLINK, SCRAPPER, SPELL_CONDUIT, SPLIT, WARBOUND, WARBOUND_BOOST, WOLFBORN</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>BUCKET_012</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>11</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>BANE_IN_MELEE_AURA, HIT_RUN_FIGHTER_AURA, MELEE_EVASION_AURA, MELEE_SHROUDING_AURA, MELEE_SLAYER_AURA, RAVAGE, RENDING_IN_MELEE_AURA, SHRED_IN_MELEE_AURA, THRUST_IN_MELEE_AURA, UNPREDICTABLE_FIGHTER_AURA, UNSTOPPABLE_IN_MELEE_AURA</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>BUCKET_005</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>7</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>SURGE, BLOODBORN, BUTCHER, CLAN_WARRIOR, FEROCIOUS, PRIMAL, SLASH</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>sixes_rolled</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>AFTER_HIT</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>unmodified_6_hit</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>BUCKET_035</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>6</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>DECIMATE, DEMOLISH, DISINTEGRATE, REAP, SCRATCH, SHATTER</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CALC_AP</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>BUCKET_019</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>BLOOD_TRAUMA, CEREBRAL_TRAUMA, DARK_TRAUMA, KNIGHT_TRAUMA, WATCH_TRAUMA, WOLF_TRAUMA</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1 hits, with Smash</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>BUCKET_020</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>6</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>BLOOD_WOUND, DARK_WOUND, KNIGHT_WOUND, MIND_WOUND, WATCH_WOUND, WOLF_WOUND</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2 hits, with Demolish</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>BUCKET_018</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>6</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>BLOOD_DOME, DARK_DOME, KNIGHT_DOME, PROTECTIVE_DOME, WATCH_DOME, WOLF_DOME</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Evasive</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>BUCKET_008</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>6</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>ADVANCED_SIGHT, BLOOD_SIGHT, DARK_SIGHT, KNIGHT_SIGHT, WATCH_SIGHT, WOLF_SIGHT</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Unstoppable</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>BUCKET_046</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>FLAME_BOTS, HAVOC_TERROR, LIGHTNING_FOG, MUTATING_INFERNO, PIRANHA_CURSE</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>4 hits, each</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>BUCKET_010</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>AMMO_BOOST, AURA_OF_PESTILENCE, CASTER_GROUP, CURSED_STRIDE, WEAPON_BOOSTER</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>BUCKET_044</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>5</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>FAST_AURA, HIGHBORN, LUSTBOUND_BOOST, SCURRY, SHOCK_SPEED</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>AIRCRAFT</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Aircraft</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>AIRCRAFT</t>
+        </is>
+      </c>
+      <c r="D507" t="inlineStr">
         <is>
           <t>MOVEMENT</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>BUCKET_056</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>4</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>JAGUAR_BLAZE, MIND_GASH, OVERPOWERING_LASH, SHIELD_BREAKER</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>6 hits, with AP (1) and Shred</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>BUCKET_058</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>KNIGHTBORN, PLAGUEBOUND, PLAGUEBOUND_BOOST, SELF_REPAIR</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
+      <c r="E507" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F507" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G507" t="inlineStr">
+        <is>
+          <t>unit_type</t>
+        </is>
+      </c>
+      <c r="H507" t="inlineStr">
+        <is>
+          <t>aircraft</t>
+        </is>
+      </c>
+      <c r="I507" t="inlineStr"/>
+      <c r="J507" t="inlineStr"/>
+      <c r="K507" t="inlineStr"/>
+      <c r="L507" t="inlineStr"/>
+      <c r="M507" t="inlineStr"/>
+      <c r="N507" t="inlineStr"/>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>ARMOR</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Armor(X)</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>ARMOR</t>
+        </is>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>DEF_ROLL</t>
+        </is>
+      </c>
+      <c r="E508" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F508" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G508" t="inlineStr">
+        <is>
+          <t>armor_value</t>
+        </is>
+      </c>
+      <c r="H508" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I508" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J508" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K508" t="inlineStr"/>
+      <c r="L508" t="inlineStr"/>
+      <c r="M508" t="inlineStr"/>
+      <c r="N508" t="inlineStr"/>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>ARTILLERY</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Artillery</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>ARTILLERY</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>TARGETING</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F509" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G509" t="inlineStr">
+        <is>
+          <t>unit_type</t>
+        </is>
+      </c>
+      <c r="H509" t="inlineStr">
+        <is>
+          <t>artillery</t>
+        </is>
+      </c>
+      <c r="I509" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J509" t="inlineStr"/>
+      <c r="K509" t="inlineStr"/>
+      <c r="L509" t="inlineStr"/>
+      <c r="M509" t="inlineStr"/>
+      <c r="N509" t="inlineStr"/>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>ENERGY_SHIELD</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Energy Shield</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>REGENERATION</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>DEF_ROLL</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F510" t="inlineStr">
         <is>
           <t>ROLL</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>6+</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
+      <c r="G510" t="inlineStr">
+        <is>
+          <t>ignore_wound</t>
+        </is>
+      </c>
+      <c r="H510" t="inlineStr">
+        <is>
+          <t>5+</t>
+        </is>
+      </c>
+      <c r="I510" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J510" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K510" t="inlineStr"/>
+      <c r="L510" t="inlineStr"/>
+      <c r="M510" t="inlineStr"/>
+      <c r="N510" t="inlineStr"/>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>IGNORES_COVER_WHEN_SHOOTING</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Ignores Cover when Shooting</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>BUCKET_003</t>
+        </is>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>DEF_ROLL</t>
+        </is>
+      </c>
+      <c r="E511" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F511" t="inlineStr">
+        <is>
+          <t>NEGATE</t>
+        </is>
+      </c>
+      <c r="G511" t="inlineStr">
+        <is>
+          <t>cover_bonus</t>
+        </is>
+      </c>
+      <c r="H511" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I511" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J511" t="inlineStr"/>
+      <c r="K511" t="inlineStr"/>
+      <c r="L511" t="inlineStr"/>
+      <c r="M511" t="inlineStr"/>
+      <c r="N511" t="inlineStr"/>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>IGNORES_REGENERATION_IN_MELEE</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Ignores Regeneration in Melee</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>BUCKET_002</t>
+        </is>
+      </c>
+      <c r="D512" t="inlineStr">
         <is>
           <t>REGEN</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>BUCKET_016</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>4</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>BIO_HORROR, MIND_BREAKER, MIND_CORRUPTION, ZAP</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2 hits, with AP (1) and Surge</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>BUCKET_009</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>4</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>AMBUSH_AURA, AMBUSH_BEACON, INFILTRATE, REPEL_AMBUSHERS</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
+      <c r="E512" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F512" t="inlineStr">
+        <is>
+          <t>NEGATE</t>
+        </is>
+      </c>
+      <c r="G512" t="inlineStr">
+        <is>
+          <t>regeneration</t>
+        </is>
+      </c>
+      <c r="H512" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I512" t="inlineStr"/>
+      <c r="J512" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K512" t="inlineStr"/>
+      <c r="L512" t="inlineStr"/>
+      <c r="M512" t="inlineStr"/>
+      <c r="N512" t="inlineStr"/>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>IMMOBILE</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Immobile</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>IMMOBILE</t>
+        </is>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>MOVEMENT</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F513" t="inlineStr">
         <is>
           <t>SET</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>reserve</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
+      <c r="G513" t="inlineStr">
+        <is>
+          <t>move_distance</t>
+        </is>
+      </c>
+      <c r="H513" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I513" t="inlineStr"/>
+      <c r="J513" t="inlineStr"/>
+      <c r="K513" t="inlineStr"/>
+      <c r="L513" t="inlineStr"/>
+      <c r="M513" t="inlineStr"/>
+      <c r="N513" t="inlineStr"/>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>MASSIVE_SPORES</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Massive Spores</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>SPORES</t>
+        </is>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>SHOOTING</t>
+        </is>
+      </c>
+      <c r="E514" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F514" t="inlineStr">
+        <is>
+          <t>SPECIAL</t>
+        </is>
+      </c>
+      <c r="G514" t="inlineStr">
+        <is>
+          <t>massive_spore_attack</t>
+        </is>
+      </c>
+      <c r="H514" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I514" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J514" t="inlineStr"/>
+      <c r="K514" t="inlineStr"/>
+      <c r="L514" t="inlineStr"/>
+      <c r="M514" t="inlineStr"/>
+      <c r="N514" t="inlineStr"/>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>PRECISION</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>SNIPER</t>
+        </is>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>TARGETING</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F515" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G515" t="inlineStr">
+        <is>
+          <t>precision_targeting</t>
+        </is>
+      </c>
+      <c r="H515" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I515" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J515" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K515" t="inlineStr"/>
+      <c r="L515" t="inlineStr"/>
+      <c r="M515" t="inlineStr"/>
+      <c r="N515" t="inlineStr"/>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>SPORES</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Spores</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>SPORES</t>
+        </is>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>SHOOTING</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F516" t="inlineStr">
+        <is>
+          <t>SPECIAL</t>
+        </is>
+      </c>
+      <c r="G516" t="inlineStr">
+        <is>
+          <t>spore_attack</t>
+        </is>
+      </c>
+      <c r="H516" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I516" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J516" t="inlineStr"/>
+      <c r="K516" t="inlineStr"/>
+      <c r="L516" t="inlineStr"/>
+      <c r="M516" t="inlineStr"/>
+      <c r="N516" t="inlineStr"/>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>TRANSPORT</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Transport(X)</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>TRANSPORT</t>
+        </is>
+      </c>
+      <c r="D517" t="inlineStr">
         <is>
           <t>DEPLOYMENT</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>BUCKET_004</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>4</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>MORALE_BOOST, COURAGE_AURA, HIVE_BOND, HOLD_THE_LINE</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>MORALE</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>BUCKET_036</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>4</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>DEEP_MEDITATION, PRECISION_SHOOTER_AURA, TARGETING_VISOR, UNPREDICTABLE_SHOOTER</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>BUCKET_045</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>FATAL_SORROW, ROT_WAVE, SEARING_BURST, SYSTEM_TAKEOVER</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>6 hits</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>BUCKET_066</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>4</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>RAPID_ADVANCE_AURA, RAPID_RUSH_AURA, STEADFAST_AURA, SWIFT</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>BUCKET_062</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>3</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>PRECISION_FIGHTER_AURA, RAIDING_DRUGS, UNPREDICTABLE_FIGHTER</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>BUCKET_037</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>3</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>DESTRUCTIVE_FRENZY, RUINOUS_FRENZY, WATCHBORN</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>BUCKET_028</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>3</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>CHANGEBOUND, CHANGEBOUND_BOOST, MACHINE_FOG</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>BUCKET_047</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>3</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>GODLY_THUNDER, PLAGUE_MALEDICTION, PSY_DESTRUCTION</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>2 hits, with AP (4)</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>BUCKET_059</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>3</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>MEND, PRECISION_SPOTTER, RE_POSITION_ARTILLERY</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>BUCKET_031</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>3</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>COORDINATED_AGGRESSION, CORRODE_WEAPONS, MOB_FRENZY</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
+      <c r="E517" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F517" t="inlineStr">
         <is>
           <t>SET</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>CALC_AP</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>BUCKET_034</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>3</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>DEATHSTRIKE, RETALIATE, SELF_DESTRUCT</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>DAMAGE</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>DIRECT_DAMAGE</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>BUCKET_030</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>CLEAVING_RUNE, CRACKLING_BOLT, SEARING_ADMONITION</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>3 hits, with Blast (3)</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>BUCKET_022</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>3</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>BRAIN_BURST, FERAL_STRIKE, VOLATILE_INFECTION</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>3 hits, with AP (2) and Deadly (3)</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>BUCKET_027</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>3</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>CASTING_BUFF, DANGEROUS_TERRAIN_DEBUFF, DIFFICULT_TERRAIN_DEBUFF</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="G517" t="inlineStr">
+        <is>
+          <t>transport_capacity</t>
+        </is>
+      </c>
+      <c r="H517" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I517" t="inlineStr"/>
+      <c r="J517" t="inlineStr"/>
+      <c r="K517" t="inlineStr"/>
+      <c r="L517" t="inlineStr"/>
+      <c r="M517" t="inlineStr"/>
+      <c r="N517" t="inlineStr"/>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>AIRCRAFT</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Aircraft</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>AIRCRAFT</t>
+        </is>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>MOVEMENT</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F518" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G518" t="inlineStr">
+        <is>
+          <t>unit_type</t>
+        </is>
+      </c>
+      <c r="H518" t="inlineStr">
+        <is>
+          <t>aircraft</t>
+        </is>
+      </c>
+      <c r="I518" t="inlineStr"/>
+      <c r="J518" t="inlineStr"/>
+      <c r="K518" t="inlineStr"/>
+      <c r="L518" t="inlineStr"/>
+      <c r="M518" t="inlineStr"/>
+      <c r="N518" t="inlineStr"/>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>ARMOR</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Armor(X)</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>ARMOR</t>
+        </is>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>DEF_ROLL</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F519" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G519" t="inlineStr">
+        <is>
+          <t>armor_value</t>
+        </is>
+      </c>
+      <c r="H519" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I519" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J519" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K519" t="inlineStr"/>
+      <c r="L519" t="inlineStr"/>
+      <c r="M519" t="inlineStr"/>
+      <c r="N519" t="inlineStr"/>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>ARTILLERY</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Artillery</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>ARTILLERY</t>
+        </is>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>TARGETING</t>
+        </is>
+      </c>
+      <c r="E520" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F520" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G520" t="inlineStr">
+        <is>
+          <t>unit_type</t>
+        </is>
+      </c>
+      <c r="H520" t="inlineStr">
+        <is>
+          <t>artillery</t>
+        </is>
+      </c>
+      <c r="I520" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J520" t="inlineStr"/>
+      <c r="K520" t="inlineStr"/>
+      <c r="L520" t="inlineStr"/>
+      <c r="M520" t="inlineStr"/>
+      <c r="N520" t="inlineStr"/>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>ENERGY_SHIELD</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Energy Shield</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>REGENERATION</t>
+        </is>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>DEF_ROLL</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F521" t="inlineStr">
+        <is>
+          <t>ROLL</t>
+        </is>
+      </c>
+      <c r="G521" t="inlineStr">
+        <is>
+          <t>ignore_wound</t>
+        </is>
+      </c>
+      <c r="H521" t="inlineStr">
+        <is>
+          <t>5+</t>
+        </is>
+      </c>
+      <c r="I521" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J521" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K521" t="inlineStr"/>
+      <c r="L521" t="inlineStr"/>
+      <c r="M521" t="inlineStr"/>
+      <c r="N521" t="inlineStr"/>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>IGNORES_COVER_WHEN_SHOOTING</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Ignores Cover when Shooting</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
         <is>
           <t>BUCKET_003</t>
         </is>
       </c>
-      <c r="B33" t="n">
-        <v>3</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>INDIRECT, IGNORES_COVER_AURA, IGNORES_COVER_WHEN_SHOOTING_AURA</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>DEF_ROLL</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F522" t="inlineStr">
         <is>
           <t>NEGATE</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="G522" t="inlineStr">
+        <is>
+          <t>cover_bonus</t>
+        </is>
+      </c>
+      <c r="H522" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>DEF_ROLL</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>BUCKET_006</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>3</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>SCOUT, INFILTRATE_AURA, SCOUT_AURA</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
+      <c r="I522" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J522" t="inlineStr"/>
+      <c r="K522" t="inlineStr"/>
+      <c r="L522" t="inlineStr"/>
+      <c r="M522" t="inlineStr"/>
+      <c r="N522" t="inlineStr"/>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>IGNORES_REGENERATION_IN_MELEE</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Ignores Regeneration in Melee</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>BUCKET_002</t>
+        </is>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>REGEN</t>
+        </is>
+      </c>
+      <c r="E523" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F523" t="inlineStr">
+        <is>
+          <t>NEGATE</t>
+        </is>
+      </c>
+      <c r="G523" t="inlineStr">
+        <is>
+          <t>regeneration</t>
+        </is>
+      </c>
+      <c r="H523" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I523" t="inlineStr"/>
+      <c r="J523" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K523" t="inlineStr"/>
+      <c r="L523" t="inlineStr"/>
+      <c r="M523" t="inlineStr"/>
+      <c r="N523" t="inlineStr"/>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>IMMOBILE</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Immobile</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>IMMOBILE</t>
+        </is>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>MOVEMENT</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F524" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G524" t="inlineStr">
+        <is>
+          <t>move_distance</t>
+        </is>
+      </c>
+      <c r="H524" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I524" t="inlineStr"/>
+      <c r="J524" t="inlineStr"/>
+      <c r="K524" t="inlineStr"/>
+      <c r="L524" t="inlineStr"/>
+      <c r="M524" t="inlineStr"/>
+      <c r="N524" t="inlineStr"/>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>MASSIVE_SPORES</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Massive Spores</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>SPORES</t>
+        </is>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>SHOOTING</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F525" t="inlineStr">
+        <is>
+          <t>SPECIAL</t>
+        </is>
+      </c>
+      <c r="G525" t="inlineStr">
+        <is>
+          <t>massive_spore_attack</t>
+        </is>
+      </c>
+      <c r="H525" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I525" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J525" t="inlineStr"/>
+      <c r="K525" t="inlineStr"/>
+      <c r="L525" t="inlineStr"/>
+      <c r="M525" t="inlineStr"/>
+      <c r="N525" t="inlineStr"/>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>PRECISION</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>SNIPER</t>
+        </is>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>TARGETING</t>
+        </is>
+      </c>
+      <c r="E526" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F526" t="inlineStr">
+        <is>
+          <t>SET</t>
+        </is>
+      </c>
+      <c r="G526" t="inlineStr">
+        <is>
+          <t>precision_targeting</t>
+        </is>
+      </c>
+      <c r="H526" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I526" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J526" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="K526" t="inlineStr"/>
+      <c r="L526" t="inlineStr"/>
+      <c r="M526" t="inlineStr"/>
+      <c r="N526" t="inlineStr"/>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>SPORES</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Spores</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>SPORES</t>
+        </is>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>SHOOTING</t>
+        </is>
+      </c>
+      <c r="E527" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F527" t="inlineStr">
+        <is>
+          <t>SPECIAL</t>
+        </is>
+      </c>
+      <c r="G527" t="inlineStr">
+        <is>
+          <t>spore_attack</t>
+        </is>
+      </c>
+      <c r="H527" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="I527" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="J527" t="inlineStr"/>
+      <c r="K527" t="inlineStr"/>
+      <c r="L527" t="inlineStr"/>
+      <c r="M527" t="inlineStr"/>
+      <c r="N527" t="inlineStr"/>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>TRANSPORT</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Transport(X)</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>TRANSPORT</t>
+        </is>
+      </c>
+      <c r="D528" t="inlineStr">
         <is>
           <t>DEPLOYMENT</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>BUCKET_023</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>3</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>BREAK, CRACK, FRACTURE</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>AFTER_HIT</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>unmodified_6_hit</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>BUCKET_002</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>2</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>BANE, QUAKE</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>NEGATE</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>REGEN</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>BUCKET_001</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>2</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>PRECISE, UNPREDICTABLE</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>BUCKET_033</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>2</v>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>DEADLY_SURGE, PSYCHIC_VOMIT</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>6 hits, with Bane</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>BUCKET_032</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>2</v>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>CRUSHING_FORCE, POWER_BOLT</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>6 hits, with AP (2)</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>BUCKET_024</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>2</v>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>BREAKING_RUNE, RIGHTEOUS_WRATH</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>1 hits, with AP (4)</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>BUCKET_011</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>2</v>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>ART_OF_PAIN, DOOM_STRIKE</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>2 hits, with AP (2) and Deadly (3)</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>BUCKET_015</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>2</v>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>BASH, THRASH</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>MULTIPLY</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>AFTER_HIT</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>BUCKET_017</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>2</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>BLISSFUL_DANCE, FIERY_PROTECTION</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Melee Evasion</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>BUCKET_014</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>2</v>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>BANISHING_SIGIL, TECH_SICKNESS</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>DEF_ROLL</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>BUCKET_007</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>2</v>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>MELEE_EVASION, MELEE_SHROUDING</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>phase_is_melee</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>BUCKET_025</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>2</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>BURN_THE_HERETIC, SHIFTING_FORM</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>-3 to casting rolls</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>BUCKET_026</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>2</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>BURST_OF_RAGE, FATEFUL_GUIDANCE</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Furious</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>BUCKET_042</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>2</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>EVASIVE, GROUNDED_STEALTH</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>BUCKET_041</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>2</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>ENHANCE_SERUM, RAPID_MUTATION</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Regeneration</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>BUCKET_040</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>2</v>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>ELEMENTAL_SEEKER, FLAME_OF_DESTRUCTION</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>1 hits, with Blast (3)</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>BUCKET_038</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>2</v>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>DEVASTATING_FRENZY, SHROUD_FIELD</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>DEF_ROLL</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>BUCKET_050</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>2</v>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>HAVOC_TRAUMA, PIERCING_BOTS</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>2 hits, with AP (2)</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>BUCKET_049</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>2</v>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>GUERRILLA, HARASSING</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>BUCKET_048</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>2</v>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>GUARDIAN, REINFORCED</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
+      <c r="E528" t="inlineStr">
+        <is>
+          <t>always</t>
+        </is>
+      </c>
+      <c r="F528" t="inlineStr">
         <is>
           <t>SET</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>CALC_AP</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>BUCKET_043</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>2</v>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>EXPEL_THREAT, HIVE_SHRIEK</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>6 hits, with AP (1)</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>BUCKET_039</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>2</v>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>DRAGON_BREATH, HOLISTIC_SUFFERING</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>9 hits</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>BUCKET_054</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>2</v>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>IMPALE, SKEWER</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>MULTIPLY</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>AFTER_WOUND</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>BUCKET_051</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>2</v>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>HEADTAKER_STRIKE, PURGE_THE_IMPURE</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>3 hits, with AP (2) each</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>BUCKET_052</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>2</v>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>HEAVENLY_LANCE, TOTAL_SEIZURE</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>4 hits, with AP (1)</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>BUCKET_057</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>2</v>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>KILLING_BLOW, POWER_BEAM</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>DEAL_HITS</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>2 hits, with AP (1)</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>ACTIVATION_START</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>BUCKET_055</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>2</v>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>INQUISITORIAL_AGENT, MARTIAL_PROWESS</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>once_per_game</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>BUCKET_053</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>2</v>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>HONOR_CODE, STEADFAST</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>BUCKET_060</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>2</v>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>MIND_SHAPER, TERRIFYING_FURY</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>GRANT</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>PRE_ATTACK</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>BUCKET_061</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>2</v>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>PIERCING_SHOOTING_DEBUFF, PIERCING_SHOOTING_MARK</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>CALC_AP</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>BUCKET_063</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>2</v>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>PRECISION_FIGHTER_BUFF, PRECISION_FIGHTING_MARK</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>SHT=, MEL=Y, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>BUCKET_064</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>2</v>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>PRECISION_SHOOTER_BUFF, PRECISION_SHOOTING_MARK</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>HIT_ROLL</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>once_per_activation</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=, CHG=</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>BUCKET_065</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>2</v>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>PUNCTURE, TEAR</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>ADD</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>CALC_AP</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>always</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>SHT=Y, MEL=Y, CHG=</t>
-        </is>
-      </c>
+      <c r="G528" t="inlineStr">
+        <is>
+          <t>transport_capacity</t>
+        </is>
+      </c>
+      <c r="H528" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="I528" t="inlineStr"/>
+      <c r="J528" t="inlineStr"/>
+      <c r="K528" t="inlineStr"/>
+      <c r="L528" t="inlineStr"/>
+      <c r="M528" t="inlineStr"/>
+      <c r="N528" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>